<commit_message>
Added a register for silo full (TO BE IMPLEMENTED)
</commit_message>
<xml_diff>
--- a/Registros.xlsx
+++ b/Registros.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t>Numero</t>
   </si>
@@ -255,6 +255,9 @@
   </si>
   <si>
     <t>Cable 7 - Sensor 7 temperature last reading</t>
+  </si>
+  <si>
+    <t>Silo full signal</t>
   </si>
 </sst>
 </file>
@@ -286,7 +289,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -361,36 +364,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -427,7 +400,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -442,19 +415,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -738,10 +705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C75"/>
+  <dimension ref="A1:C76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E67" sqref="E67"/>
+      <selection activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -752,25 +719,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="7">
+      <c r="A2" s="5">
         <v>0</v>
       </c>
-      <c r="B2" s="9" t="str">
+      <c r="B2" s="7" t="str">
         <f>DEC2HEX(A2,2)</f>
         <v>00</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="8" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1547,7 +1514,7 @@
         <v>65</v>
       </c>
       <c r="B67" s="2" t="str">
-        <f t="shared" ref="B67:B75" si="1">DEC2HEX(A67,2)</f>
+        <f t="shared" ref="B67:B76" si="1">DEC2HEX(A67,2)</f>
         <v>41</v>
       </c>
       <c r="C67" s="4" t="s">
@@ -1638,16 +1605,28 @@
         <v>75</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="5">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" s="3">
         <v>73</v>
       </c>
-      <c r="B75" s="6" t="str">
+      <c r="B75" s="2" t="str">
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>76</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" s="3">
+        <v>74</v>
+      </c>
+      <c r="B76" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>4A</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added take reading trigger register (0x02)
</commit_message>
<xml_diff>
--- a/Registros.xlsx
+++ b/Registros.xlsx
@@ -1,30 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giuliano.OMBUSA\Documents\MPLABX_Projects\umt-modbus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giuli\Desktop\Dascanio\umt-modbus\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{ED726093-C7F7-421C-8087-4E28C988490D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
   <si>
     <t>Numero</t>
   </si>
@@ -261,12 +268,15 @@
   </si>
   <si>
     <t>Timeout between readings seconds (60&lt;= x &lt;= 21600)</t>
+  </si>
+  <si>
+    <t>Start a reading if set &gt;0 (cleared by soft)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -689,14 +699,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C77"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.5546875" style="1"/>
     <col min="2" max="2" width="13.21875" style="1" customWidth="1"/>
@@ -731,7 +741,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="str">
-        <f t="shared" ref="B3:B4" si="0">DEC2HEX(A3,2)</f>
+        <f>DEC2HEX(A3,2)</f>
         <v>01</v>
       </c>
       <c r="C3" s="7" t="s">
@@ -743,23 +753,23 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>DEC2HEX(A4,2)</f>
         <v>02</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="str">
-        <f t="shared" ref="B5:B68" si="1">DEC2HEX(A5,2)</f>
+      <c r="B5" s="6" t="str">
+        <f>DEC2HEX(A5,2)</f>
         <v>03</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>4</v>
+      <c r="C5" s="7" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -767,11 +777,11 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="B6:B69" si="0">DEC2HEX(A6,2)</f>
         <v>04</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -779,11 +789,11 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>05</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -791,11 +801,11 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>06</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -803,11 +813,11 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>07</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -815,11 +825,11 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>08</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -827,11 +837,11 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>09</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -839,11 +849,11 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0A</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -851,11 +861,11 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0B</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -863,11 +873,11 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0C</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -875,11 +885,11 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0D</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -887,11 +897,11 @@
         <v>14</v>
       </c>
       <c r="B16" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0E</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -899,11 +909,11 @@
         <v>15</v>
       </c>
       <c r="B17" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0F</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -911,11 +921,11 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -923,11 +933,11 @@
         <v>17</v>
       </c>
       <c r="B19" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -935,11 +945,11 @@
         <v>18</v>
       </c>
       <c r="B20" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -947,11 +957,11 @@
         <v>19</v>
       </c>
       <c r="B21" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -959,11 +969,11 @@
         <v>20</v>
       </c>
       <c r="B22" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -971,11 +981,11 @@
         <v>21</v>
       </c>
       <c r="B23" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -983,11 +993,11 @@
         <v>22</v>
       </c>
       <c r="B24" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -995,11 +1005,11 @@
         <v>23</v>
       </c>
       <c r="B25" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -1007,11 +1017,11 @@
         <v>24</v>
       </c>
       <c r="B26" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -1019,11 +1029,11 @@
         <v>25</v>
       </c>
       <c r="B27" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -1031,11 +1041,11 @@
         <v>26</v>
       </c>
       <c r="B28" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1A</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -1043,11 +1053,11 @@
         <v>27</v>
       </c>
       <c r="B29" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1B</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -1055,11 +1065,11 @@
         <v>28</v>
       </c>
       <c r="B30" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1C</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -1067,11 +1077,11 @@
         <v>29</v>
       </c>
       <c r="B31" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1D</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -1079,11 +1089,11 @@
         <v>30</v>
       </c>
       <c r="B32" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1E</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -1091,11 +1101,11 @@
         <v>31</v>
       </c>
       <c r="B33" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1F</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
@@ -1103,11 +1113,11 @@
         <v>32</v>
       </c>
       <c r="B34" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
@@ -1115,11 +1125,11 @@
         <v>33</v>
       </c>
       <c r="B35" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -1127,11 +1137,11 @@
         <v>34</v>
       </c>
       <c r="B36" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
@@ -1139,11 +1149,11 @@
         <v>35</v>
       </c>
       <c r="B37" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
@@ -1151,11 +1161,11 @@
         <v>36</v>
       </c>
       <c r="B38" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -1163,11 +1173,11 @@
         <v>37</v>
       </c>
       <c r="B39" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -1175,11 +1185,11 @@
         <v>38</v>
       </c>
       <c r="B40" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -1187,11 +1197,11 @@
         <v>39</v>
       </c>
       <c r="B41" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -1199,11 +1209,11 @@
         <v>40</v>
       </c>
       <c r="B42" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
@@ -1211,11 +1221,11 @@
         <v>41</v>
       </c>
       <c r="B43" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
@@ -1223,11 +1233,11 @@
         <v>42</v>
       </c>
       <c r="B44" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2A</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
@@ -1235,11 +1245,11 @@
         <v>43</v>
       </c>
       <c r="B45" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2B</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
@@ -1247,11 +1257,11 @@
         <v>44</v>
       </c>
       <c r="B46" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2C</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
@@ -1259,11 +1269,11 @@
         <v>45</v>
       </c>
       <c r="B47" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2D</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
@@ -1271,11 +1281,11 @@
         <v>46</v>
       </c>
       <c r="B48" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2E</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
@@ -1283,11 +1293,11 @@
         <v>47</v>
       </c>
       <c r="B49" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2F</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
@@ -1295,11 +1305,11 @@
         <v>48</v>
       </c>
       <c r="B50" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
@@ -1307,11 +1317,11 @@
         <v>49</v>
       </c>
       <c r="B51" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
@@ -1319,11 +1329,11 @@
         <v>50</v>
       </c>
       <c r="B52" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
@@ -1331,11 +1341,11 @@
         <v>51</v>
       </c>
       <c r="B53" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
@@ -1343,11 +1353,11 @@
         <v>52</v>
       </c>
       <c r="B54" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
@@ -1355,11 +1365,11 @@
         <v>53</v>
       </c>
       <c r="B55" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
@@ -1367,11 +1377,11 @@
         <v>54</v>
       </c>
       <c r="B56" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
@@ -1379,11 +1389,11 @@
         <v>55</v>
       </c>
       <c r="B57" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
@@ -1391,11 +1401,11 @@
         <v>56</v>
       </c>
       <c r="B58" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>38</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
@@ -1403,11 +1413,11 @@
         <v>57</v>
       </c>
       <c r="B59" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>39</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
@@ -1415,11 +1425,11 @@
         <v>58</v>
       </c>
       <c r="B60" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3A</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
@@ -1427,11 +1437,11 @@
         <v>59</v>
       </c>
       <c r="B61" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3B</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
@@ -1439,11 +1449,11 @@
         <v>60</v>
       </c>
       <c r="B62" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3C</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
@@ -1451,11 +1461,11 @@
         <v>61</v>
       </c>
       <c r="B63" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3D</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
@@ -1463,11 +1473,11 @@
         <v>62</v>
       </c>
       <c r="B64" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3E</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
@@ -1475,11 +1485,11 @@
         <v>63</v>
       </c>
       <c r="B65" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3F</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
@@ -1487,11 +1497,11 @@
         <v>64</v>
       </c>
       <c r="B66" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
@@ -1499,11 +1509,11 @@
         <v>65</v>
       </c>
       <c r="B67" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
@@ -1511,11 +1521,11 @@
         <v>66</v>
       </c>
       <c r="B68" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>42</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
@@ -1523,11 +1533,11 @@
         <v>67</v>
       </c>
       <c r="B69" s="2" t="str">
-        <f t="shared" ref="B69:B77" si="2">DEC2HEX(A69,2)</f>
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
@@ -1535,11 +1545,11 @@
         <v>68</v>
       </c>
       <c r="B70" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="B70:B78" si="1">DEC2HEX(A70,2)</f>
         <v>44</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
@@ -1547,11 +1557,11 @@
         <v>69</v>
       </c>
       <c r="B71" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
@@ -1559,11 +1569,11 @@
         <v>70</v>
       </c>
       <c r="B72" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
@@ -1571,11 +1581,11 @@
         <v>71</v>
       </c>
       <c r="B73" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>47</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
@@ -1583,11 +1593,11 @@
         <v>72</v>
       </c>
       <c r="B74" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>48</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
@@ -1595,11 +1605,11 @@
         <v>73</v>
       </c>
       <c r="B75" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>49</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
@@ -1607,11 +1617,11 @@
         <v>74</v>
       </c>
       <c r="B76" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4A</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
@@ -1619,10 +1629,22 @@
         <v>75</v>
       </c>
       <c r="B77" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4B</v>
       </c>
       <c r="C77" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" s="4">
+        <v>76</v>
+      </c>
+      <c r="B78" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>4C</v>
+      </c>
+      <c r="C78" s="3" t="s">
         <v>76</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed temperature variable to be a signed integer, so values could be easily convert on TC1000 later
</commit_message>
<xml_diff>
--- a/Registros.xlsx
+++ b/Registros.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -709,7 +709,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -1665,8 +1665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D2:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1700,5 +1700,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>